<commit_message>
Trying to get web app back up
</commit_message>
<xml_diff>
--- a/example_app_tracker.xlsx
+++ b/example_app_tracker.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graha\OneDrive\Documents\GitHub\application_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2637769-1386-4DE7-B0FF-9CB2C521E569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E467CBE5-2312-45C0-9CD9-7849EDAB45C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18010" yWindow="3980" windowWidth="20070" windowHeight="15190" activeTab="2" xr2:uid="{85E7A6A4-6F22-48D9-815F-FC03736B7AC4}"/>
+    <workbookView xWindow="17350" yWindow="5010" windowWidth="20070" windowHeight="15190" activeTab="1" xr2:uid="{85E7A6A4-6F22-48D9-815F-FC03736B7AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="Interviews" sheetId="6" r:id="rId2"/>
     <sheet name="ROE Calculation" sheetId="4" r:id="rId3"/>
     <sheet name="Glossary" sheetId="5" r:id="rId4"/>
   </sheets>
@@ -1529,11 +1529,11 @@
       </c>
       <c r="G2">
         <f ca="1">ROUND(RAND()*60+50,0)</f>
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="H2">
         <f ca="1">ROUND(RAND()*40+100,0)</f>
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
@@ -1567,11 +1567,11 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G66" ca="1" si="1">ROUND(RAND()*60+50,0)</f>
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H66" ca="1" si="2">ROUND(RAND()*40+100,0)</f>
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
@@ -1605,11 +1605,11 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="2"/>
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
@@ -1643,11 +1643,11 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="2"/>
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>10</v>
@@ -1681,11 +1681,11 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="2"/>
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
@@ -1719,11 +1719,11 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="2"/>
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
@@ -1757,11 +1757,11 @@
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="2"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
@@ -1795,11 +1795,11 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="2"/>
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
@@ -1833,11 +1833,11 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="2"/>
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>13</v>
@@ -1871,11 +1871,11 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="2"/>
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
@@ -1909,11 +1909,11 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="2"/>
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
@@ -1947,11 +1947,11 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="2"/>
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>10</v>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="2"/>
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>10</v>
@@ -2023,11 +2023,11 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="2"/>
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>10</v>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="2"/>
@@ -2099,11 +2099,11 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="2"/>
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>14</v>
@@ -2137,11 +2137,11 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>14</v>
@@ -2175,11 +2175,11 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="2"/>
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>14</v>
@@ -2213,11 +2213,11 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="2"/>
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>14</v>
@@ -2251,11 +2251,11 @@
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="2"/>
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>214</v>
@@ -2289,11 +2289,11 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="2"/>
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>214</v>
@@ -2327,11 +2327,11 @@
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="2"/>
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>214</v>
@@ -2365,11 +2365,11 @@
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>9</v>
@@ -2403,11 +2403,11 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="2"/>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>9</v>
@@ -2441,11 +2441,11 @@
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="2"/>
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>9</v>
@@ -2479,11 +2479,11 @@
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="2"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>9</v>
@@ -2517,11 +2517,11 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="2"/>
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>9</v>
@@ -2555,11 +2555,11 @@
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="2"/>
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>9</v>
@@ -2593,11 +2593,11 @@
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="2"/>
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>9</v>
@@ -2631,11 +2631,11 @@
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="2"/>
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>9</v>
@@ -2669,11 +2669,11 @@
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>14</v>
@@ -2707,11 +2707,11 @@
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="2"/>
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>15</v>
@@ -2745,11 +2745,11 @@
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="2"/>
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>15</v>
@@ -2783,11 +2783,11 @@
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="2"/>
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>15</v>
@@ -2821,11 +2821,11 @@
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="2"/>
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>15</v>
@@ -2859,11 +2859,11 @@
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="2"/>
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>17</v>
@@ -2897,11 +2897,11 @@
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="2"/>
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>17</v>
@@ -2935,11 +2935,11 @@
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="2"/>
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>17</v>
@@ -2973,11 +2973,11 @@
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="2"/>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>17</v>
@@ -3011,11 +3011,11 @@
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="2"/>
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>17</v>
@@ -3049,11 +3049,11 @@
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="2"/>
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>17</v>
@@ -3087,11 +3087,11 @@
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="1"/>
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="2"/>
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>17</v>
@@ -3125,11 +3125,11 @@
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="2"/>
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>18</v>
@@ -3163,11 +3163,11 @@
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="1"/>
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="2"/>
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>18</v>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="2"/>
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>18</v>
@@ -3239,11 +3239,11 @@
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="2"/>
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>18</v>
@@ -3277,11 +3277,11 @@
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="2"/>
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>18</v>
@@ -3315,11 +3315,11 @@
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="2"/>
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>18</v>
@@ -3353,11 +3353,11 @@
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="2"/>
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>18</v>
@@ -3391,11 +3391,11 @@
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="2"/>
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>33</v>
@@ -3429,11 +3429,11 @@
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="2"/>
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>33</v>
@@ -3467,11 +3467,11 @@
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="2"/>
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>33</v>
@@ -3505,11 +3505,11 @@
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="2"/>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>33</v>
@@ -3543,11 +3543,11 @@
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="2"/>
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>33</v>
@@ -3581,11 +3581,11 @@
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="2"/>
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>33</v>
@@ -3619,11 +3619,11 @@
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="2"/>
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>33</v>
@@ -3657,11 +3657,11 @@
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="2"/>
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>33</v>
@@ -3695,11 +3695,11 @@
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="2"/>
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>33</v>
@@ -3733,11 +3733,11 @@
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="2"/>
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>34</v>
@@ -3771,11 +3771,11 @@
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="2"/>
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>34</v>
@@ -3809,11 +3809,11 @@
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="2"/>
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>34</v>
@@ -3847,11 +3847,11 @@
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="1"/>
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="2"/>
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>34</v>
@@ -3885,11 +3885,11 @@
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="2"/>
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>34</v>
@@ -3923,11 +3923,11 @@
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="2"/>
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>34</v>
@@ -3961,11 +3961,11 @@
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="2"/>
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>11</v>
@@ -3999,11 +3999,11 @@
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G75" ca="1" si="5">ROUND(RAND()*60+50,0)</f>
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H75" ca="1" si="6">ROUND(RAND()*40+100,0)</f>
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>11</v>
@@ -4037,11 +4037,11 @@
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="5"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="6"/>
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>11</v>
@@ -4075,11 +4075,11 @@
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="5"/>
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="6"/>
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>11</v>
@@ -4113,11 +4113,11 @@
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="5"/>
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="6"/>
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>11</v>
@@ -4151,11 +4151,11 @@
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="5"/>
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="6"/>
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>9</v>
@@ -4189,11 +4189,11 @@
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="5"/>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="6"/>
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>9</v>
@@ -4227,11 +4227,11 @@
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="5"/>
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="6"/>
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>9</v>
@@ -4265,11 +4265,11 @@
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="5"/>
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="6"/>
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>9</v>
@@ -4303,11 +4303,11 @@
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="6"/>
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>9</v>
@@ -4399,7 +4399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E6A88D-3241-41C0-B7E9-472CCE1959EA}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -4881,7 +4881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70590CAF-D2CD-443E-AE13-8F53684D3C03}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
@@ -4948,7 +4948,7 @@
       </c>
       <c r="D2">
         <f ca="1">(Tracker!G2+Tracker!H2)/2</f>
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E2" s="10">
         <f>IF(OR(Tracker!F2="denied",Tracker!F2="on hold",Tracker!F2="No Response",Tracker!F2="pending",Tracker!F26="ghosted"), 0.2, IF(Tracker!F2="interviewing", 0.4, IF(Tracker!F2="rejected", 0.3, IF(Tracker!F2="offer", 1, 0))))</f>
@@ -4971,11 +4971,11 @@
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J15" ca="1" si="0">IF(D2=0,0,((0.3*D2*G2*H2)/10)-2.7)</f>
-        <v>9.0149999999999508E-2</v>
+        <v>0.84254999999999969</v>
       </c>
       <c r="K2">
         <f t="shared" ref="K2:K15" ca="1" si="1">IF(D2=0, 0,((D2*E2*G2*H2)/(F2*I2)-2))</f>
-        <v>0.17555555555555546</v>
+        <v>0.76222222222222191</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -4993,7 +4993,7 @@
       </c>
       <c r="D3">
         <f ca="1">(Tracker!G3+Tracker!H3)/2</f>
-        <v>109.5</v>
+        <v>104.5</v>
       </c>
       <c r="E3" s="10">
         <f>IF(OR(Tracker!F3="denied",Tracker!F3="on hold",Tracker!F3="No Response",Tracker!F3="pending",Tracker!F27="ghosted"), 0.2, IF(Tracker!F3="interviewing", 0.4, IF(Tracker!F3="rejected", 0.3, IF(Tracker!F3="offer", 1, 0))))</f>
@@ -5016,11 +5016,11 @@
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73282500000000006</v>
+        <v>0.57607499999999945</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4873529411764705</v>
+        <v>2.2824509803921558</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="D4">
         <f ca="1">(Tracker!G4+Tracker!H4)/2</f>
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E4" s="10">
         <f>IF(OR(Tracker!F4="denied",Tracker!F4="on hold",Tracker!F4="No Response",Tracker!F4="pending",Tracker!F28="ghosted"), 0.2, IF(Tracker!F4="interviewing", 0.4, IF(Tracker!F4="rejected", 0.3, IF(Tracker!F4="offer", 1, 0))))</f>
@@ -5061,11 +5061,11 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77985000000000015</v>
+        <v>0.56039999999999957</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57766666666666744</v>
+        <v>0.41511111111111099</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -5083,7 +5083,7 @@
       </c>
       <c r="D5">
         <f ca="1">(Tracker!G5+Tracker!H5)/2</f>
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E5" s="10">
         <f>IF(OR(Tracker!F5="denied",Tracker!F5="on hold",Tracker!F5="No Response",Tracker!F5="pending",Tracker!F29="ghosted"), 0.2, IF(Tracker!F5="interviewing", 0.4, IF(Tracker!F5="rejected", 0.3, IF(Tracker!F5="offer", 1, 0))))</f>
@@ -5106,11 +5106,11 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10650000000000048</v>
+        <v>3.5999999999999588E-2</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73</v>
+        <v>0.87999999999999945</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -5128,7 +5128,7 @@
       </c>
       <c r="D6">
         <f ca="1">(Tracker!G6+Tracker!H6)/2</f>
-        <v>118.5</v>
+        <v>111.5</v>
       </c>
       <c r="E6" s="10">
         <f>IF(OR(Tracker!F6="denied",Tracker!F6="on hold",Tracker!F6="No Response",Tracker!F6="pending",Tracker!F30="ghosted"), 0.2, IF(Tracker!F6="interviewing", 0.4, IF(Tracker!F6="rejected", 0.3, IF(Tracker!F6="offer", 1, 0))))</f>
@@ -5151,11 +5151,11 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0149749999999997</v>
+        <v>0.79552499999999959</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7518333333333338</v>
+        <v>0.58927777777777779</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="D7">
         <f ca="1">(Tracker!G7+Tracker!H7)/2</f>
-        <v>89</v>
+        <v>115.5</v>
       </c>
       <c r="E7" s="10">
         <f>IF(OR(Tracker!F7="denied",Tracker!F7="on hold",Tracker!F7="No Response",Tracker!F7="pending",Tracker!F31="ghosted"), 0.2, IF(Tracker!F7="interviewing", 0.4, IF(Tracker!F7="rejected", 0.3, IF(Tracker!F7="offer", 1, 0))))</f>
@@ -5196,11 +5196,11 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0149999999999508E-2</v>
+        <v>0.92092499999999955</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17555555555555546</v>
+        <v>0.82333333333333325</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -5218,7 +5218,7 @@
       </c>
       <c r="D8">
         <f ca="1">(Tracker!G8+Tracker!H8)/2</f>
-        <v>95</v>
+        <v>102.5</v>
       </c>
       <c r="E8" s="10">
         <f>IF(OR(Tracker!F8="denied",Tracker!F8="on hold",Tracker!F8="No Response",Tracker!F8="pending",Tracker!F32="ghosted"), 0.2, IF(Tracker!F8="interviewing", 0.4, IF(Tracker!F8="rejected", 0.3, IF(Tracker!F8="offer", 1, 0))))</f>
@@ -5241,11 +5241,11 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27824999999999989</v>
+        <v>0.51337499999999991</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20611111111111136</v>
+        <v>0.38027777777777771</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="D9">
         <f ca="1">(Tracker!G9+Tracker!H9)/2</f>
-        <v>107</v>
+        <v>90.5</v>
       </c>
       <c r="E9" s="10">
         <f>IF(OR(Tracker!F9="denied",Tracker!F9="on hold",Tracker!F9="No Response",Tracker!F9="pending",Tracker!F33="ghosted"), 0.2, IF(Tracker!F9="interviewing", 0.4, IF(Tracker!F9="rejected", 0.3, IF(Tracker!F9="offer", 1, 0))))</f>
@@ -5286,11 +5286,11 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65444999999999975</v>
+        <v>0.13717500000000005</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61555555555555586</v>
+        <v>0.21222222222222253</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -5308,7 +5308,7 @@
       </c>
       <c r="D10">
         <f ca="1">(Tracker!G10+Tracker!H10)/2</f>
-        <v>88.5</v>
+        <v>93</v>
       </c>
       <c r="E10" s="10">
         <f>IF(OR(Tracker!F10="denied",Tracker!F10="on hold",Tracker!F10="No Response",Tracker!F10="pending",Tracker!F34="ghosted"), 0.2, IF(Tracker!F10="interviewing", 0.4, IF(Tracker!F10="rejected", 0.3, IF(Tracker!F10="offer", 1, 0))))</f>
@@ -5331,11 +5331,11 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4474999999999625E-2</v>
+        <v>0.21554999999999991</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6549999999999998</v>
+        <v>0.78999999999999959</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="D11">
         <f ca="1">(Tracker!G11+Tracker!H11)/2</f>
-        <v>105.5</v>
+        <v>107.5</v>
       </c>
       <c r="E11" s="10">
         <f>IF(OR(Tracker!F11="denied",Tracker!F11="on hold",Tracker!F11="No Response",Tracker!F11="pending",Tracker!F35="ghosted"), 0.2, IF(Tracker!F11="interviewing", 0.4, IF(Tracker!F11="rejected", 0.3, IF(Tracker!F11="offer", 1, 0))))</f>
@@ -5376,11 +5376,11 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60742499999999966</v>
+        <v>0.67012500000000008</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4499444444444447</v>
+        <v>0.49638888888888921</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -5398,7 +5398,7 @@
       </c>
       <c r="D12">
         <f ca="1">(Tracker!G12+Tracker!H12)/2</f>
-        <v>104</v>
+        <v>86.5</v>
       </c>
       <c r="E12" s="10">
         <f>IF(OR(Tracker!F12="denied",Tracker!F12="on hold",Tracker!F12="No Response",Tracker!F12="pending",Tracker!F36="ghosted"), 0.2, IF(Tracker!F12="interviewing", 0.4, IF(Tracker!F12="rejected", 0.3, IF(Tracker!F12="offer", 1, 0))))</f>
@@ -5421,11 +5421,11 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56039999999999957</v>
+        <v>1.1775000000000091E-2</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6226666666666665</v>
+        <v>1.0130833333333333</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -5443,7 +5443,7 @@
       </c>
       <c r="D13">
         <f ca="1">(Tracker!G13+Tracker!H13)/2</f>
-        <v>85.5</v>
+        <v>117.5</v>
       </c>
       <c r="E13" s="10">
         <f>IF(OR(Tracker!F13="denied",Tracker!F13="on hold",Tracker!F13="No Response",Tracker!F13="pending",Tracker!F37="ghosted"), 0.2, IF(Tracker!F13="interviewing", 0.4, IF(Tracker!F13="rejected", 0.3, IF(Tracker!F13="offer", 1, 0))))</f>
@@ -5466,11 +5466,11 @@
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.957500000000012E-2</v>
+        <v>0.98362500000000042</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.21304999999999974</v>
+        <v>0.4557500000000001</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -5488,7 +5488,7 @@
       </c>
       <c r="D14">
         <f ca="1">(Tracker!G14+Tracker!H14)/2</f>
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E14" s="10">
         <f>IF(OR(Tracker!F14="denied",Tracker!F14="on hold",Tracker!F14="No Response",Tracker!F14="pending",Tracker!F38="ghosted"), 0.2, IF(Tracker!F14="interviewing", 0.4, IF(Tracker!F14="rejected", 0.3, IF(Tracker!F14="offer", 1, 0))))</f>
@@ -5511,11 +5511,11 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27539999999999942</v>
+        <v>4.4549999999999645E-2</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.6399999999999748E-2</v>
+        <v>-0.1702999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -5533,7 +5533,7 @@
       </c>
       <c r="D15">
         <f ca="1">(Tracker!G15+Tracker!H15)/2</f>
-        <v>90.5</v>
+        <v>87.5</v>
       </c>
       <c r="E15" s="10">
         <f>IF(OR(Tracker!F15="denied",Tracker!F15="on hold",Tracker!F15="No Response",Tracker!F15="pending",Tracker!F39="ghosted"), 0.2, IF(Tracker!F15="interviewing", 0.4, IF(Tracker!F15="rejected", 0.3, IF(Tracker!F15="offer", 1, 0))))</f>
@@ -5556,11 +5556,11 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.37867500000000032</v>
+        <v>-0.45562500000000039</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7377500000000001</v>
+        <v>5.4812500000000002</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -5578,7 +5578,7 @@
       </c>
       <c r="D16">
         <f ca="1">(Tracker!G16+Tracker!H16)/2</f>
-        <v>81</v>
+        <v>85.5</v>
       </c>
       <c r="E16" s="10">
         <f>IF(OR(Tracker!F16="denied",Tracker!F16="on hold",Tracker!F16="No Response",Tracker!F16="pending",Tracker!F40="ghosted"), 0.2, IF(Tracker!F16="interviewing", 0.4, IF(Tracker!F16="rejected", 0.3, IF(Tracker!F16="offer", 1, 0))))</f>
@@ -5601,11 +5601,11 @@
       </c>
       <c r="J16">
         <f t="shared" ref="J16:J70" ca="1" si="2">IF(D16=0,0,((0.3*D16*G16*H16)/10)-2.7)</f>
-        <v>-0.6223500000000004</v>
+        <v>-0.50692500000000029</v>
       </c>
       <c r="K16">
         <f t="shared" ref="K16:K70" ca="1" si="3">IF(D16=0, 0,((D16*E16*G16*H16)/(F16*I16)-2))</f>
-        <v>-0.6149</v>
+        <v>-0.53794999999999993</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -5623,7 +5623,7 @@
       </c>
       <c r="D17">
         <f ca="1">(Tracker!G17+Tracker!H17)/2</f>
-        <v>112</v>
+        <v>102.5</v>
       </c>
       <c r="E17" s="10">
         <f>IF(OR(Tracker!F17="denied",Tracker!F17="on hold",Tracker!F17="No Response",Tracker!F17="pending",Tracker!F41="ghosted"), 0.2, IF(Tracker!F17="interviewing", 0.4, IF(Tracker!F17="rejected", 0.3, IF(Tracker!F17="offer", 1, 0))))</f>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17280000000000006</v>
+        <v>-7.0875000000000465E-2</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="3"/>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="D18">
         <f ca="1">(Tracker!G18+Tracker!H18)/2</f>
-        <v>87</v>
+        <v>112.5</v>
       </c>
       <c r="E18" s="10">
         <f>IF(OR(Tracker!F18="denied",Tracker!F18="on hold",Tracker!F18="No Response",Tracker!F18="pending",Tracker!F42="ghosted"), 0.2, IF(Tracker!F18="interviewing", 0.4, IF(Tracker!F18="rejected", 0.3, IF(Tracker!F18="offer", 1, 0))))</f>
@@ -5691,11 +5691,11 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.4684500000000007</v>
+        <v>0.18562499999999993</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="3"/>
-        <v>5.4384999999999994</v>
+        <v>7.6187500000000004</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="D19">
         <f ca="1">(Tracker!G19+Tracker!H19)/2</f>
-        <v>118</v>
+        <v>111.5</v>
       </c>
       <c r="E19" s="10">
         <f>IF(OR(Tracker!F19="denied",Tracker!F19="on hold",Tracker!F19="No Response",Tracker!F19="pending",Tracker!F43="ghosted"), 0.2, IF(Tracker!F19="interviewing", 0.4, IF(Tracker!F19="rejected", 0.3, IF(Tracker!F19="offer", 1, 0))))</f>
@@ -5736,11 +5736,11 @@
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="2"/>
-        <v>0.32669999999999977</v>
+        <v>0.15997499999999931</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.24199999999999999</v>
+        <v>0.11849999999999961</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="D20">
         <f ca="1">(Tracker!G20+Tracker!H20)/2</f>
-        <v>93.5</v>
+        <v>114</v>
       </c>
       <c r="E20" s="10">
         <f>IF(OR(Tracker!F20="denied",Tracker!F20="on hold",Tracker!F20="No Response",Tracker!F20="pending",Tracker!F44="ghosted"), 0.2, IF(Tracker!F20="interviewing", 0.4, IF(Tracker!F20="rejected", 0.3, IF(Tracker!F20="offer", 1, 0))))</f>
@@ -5781,11 +5781,11 @@
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.30172500000000024</v>
+        <v>0.22409999999999952</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.40115000000000012</v>
+        <v>-5.0599999999999978E-2</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="D21">
         <f ca="1">(Tracker!G21+Tracker!H21)/2</f>
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E21" s="10">
         <f>IF(OR(Tracker!F21="denied",Tracker!F21="on hold",Tracker!F21="No Response",Tracker!F21="pending",Tracker!F45="ghosted"), 0.2, IF(Tracker!F21="interviewing", 0.4, IF(Tracker!F21="rejected", 0.3, IF(Tracker!F21="offer", 1, 0))))</f>
@@ -5826,11 +5826,11 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.41715000000000035</v>
+        <v>-0.31455000000000055</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="3"/>
-        <v>6.4550000000000001</v>
+        <v>6.8350000000000009</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="D22">
         <f ca="1">(Tracker!G22+Tracker!H22)/2</f>
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E22" s="10">
         <f>IF(OR(Tracker!F22="denied",Tracker!F22="on hold",Tracker!F22="No Response",Tracker!F22="pending",Tracker!F46="ghosted"), 0.2, IF(Tracker!F22="interviewing", 0.4, IF(Tracker!F22="rejected", 0.3, IF(Tracker!F22="offer", 1, 0))))</f>
@@ -5871,11 +5871,11 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="2"/>
-        <v>-6.7500000000002558E-3</v>
+        <v>-0.18630000000000013</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.9999999999998934E-3</v>
+        <v>-0.13800000000000012</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -5893,7 +5893,7 @@
       </c>
       <c r="D23">
         <f ca="1">(Tracker!G23+Tracker!H23)/2</f>
-        <v>98.5</v>
+        <v>97.5</v>
       </c>
       <c r="E23" s="10">
         <f>IF(OR(Tracker!F23="denied",Tracker!F23="on hold",Tracker!F23="No Response",Tracker!F23="pending",Tracker!F47="ghosted"), 0.2, IF(Tracker!F23="interviewing", 0.4, IF(Tracker!F23="rejected", 0.3, IF(Tracker!F23="offer", 1, 0))))</f>
@@ -5916,11 +5916,11 @@
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="2"/>
-        <v>0.38797499999999996</v>
+        <v>0.35662500000000019</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.815555555555556</v>
+        <v>2.7666666666666666</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -5938,7 +5938,7 @@
       </c>
       <c r="D24">
         <f ca="1">(Tracker!G24+Tracker!H24)/2</f>
-        <v>81.5</v>
+        <v>113</v>
       </c>
       <c r="E24" s="10">
         <f>IF(OR(Tracker!F24="denied",Tracker!F24="on hold",Tracker!F24="No Response",Tracker!F24="pending",Tracker!F48="ghosted"), 0.2, IF(Tracker!F24="interviewing", 0.4, IF(Tracker!F24="rejected", 0.3, IF(Tracker!F24="offer", 1, 0))))</f>
@@ -5961,11 +5961,11 @@
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.14497500000000008</v>
+        <v>0.84254999999999969</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.10738888888888853</v>
+        <v>0.62411111111111106</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -5983,7 +5983,7 @@
       </c>
       <c r="D25">
         <f ca="1">(Tracker!G25+Tracker!H25)/2</f>
-        <v>87.5</v>
+        <v>89</v>
       </c>
       <c r="E25" s="10">
         <f>IF(OR(Tracker!F25="denied",Tracker!F25="on hold",Tracker!F25="No Response",Tracker!F25="pending",Tracker!F49="ghosted"), 0.2, IF(Tracker!F25="interviewing", 0.4, IF(Tracker!F25="rejected", 0.3, IF(Tracker!F25="offer", 1, 0))))</f>
@@ -6006,11 +6006,11 @@
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="2"/>
-        <v>4.3124999999999858E-2</v>
+        <v>9.0149999999999508E-2</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1944444444444109E-2</v>
+        <v>6.6777777777778269E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -6028,7 +6028,7 @@
       </c>
       <c r="D26">
         <f ca="1">(Tracker!G26+Tracker!H26)/2</f>
-        <v>112.5</v>
+        <v>82.5</v>
       </c>
       <c r="E26" s="10">
         <f>IF(OR(Tracker!F26="denied",Tracker!F26="on hold",Tracker!F26="No Response",Tracker!F26="pending",Tracker!F50="ghosted"), 0.2, IF(Tracker!F26="interviewing", 0.4, IF(Tracker!F26="rejected", 0.3, IF(Tracker!F26="offer", 1, 0))))</f>
@@ -6051,7 +6051,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.82687499999999936</v>
+        <v>-0.11362500000000031</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="3"/>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="D27">
         <f ca="1">(Tracker!G27+Tracker!H27)/2</f>
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E27" s="10">
         <f>IF(OR(Tracker!F27="denied",Tracker!F27="on hold",Tracker!F27="No Response",Tracker!F27="pending",Tracker!F51="ghosted"), 0.2, IF(Tracker!F27="interviewing", 0.4, IF(Tracker!F27="rejected", 0.3, IF(Tracker!F27="offer", 1, 0))))</f>
@@ -6096,11 +6096,11 @@
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="2"/>
-        <v>0.40364999999999984</v>
+        <v>0.12149999999999972</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="3"/>
-        <v>0.29899999999999993</v>
+        <v>8.9999999999999858E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -6118,7 +6118,7 @@
       </c>
       <c r="D28">
         <f ca="1">(Tracker!G28+Tracker!H28)/2</f>
-        <v>113.5</v>
+        <v>95.5</v>
       </c>
       <c r="E28" s="10">
         <f>IF(OR(Tracker!F28="denied",Tracker!F28="on hold",Tracker!F28="No Response",Tracker!F28="pending",Tracker!F52="ghosted"), 0.2, IF(Tracker!F28="interviewing", 0.4, IF(Tracker!F28="rejected", 0.3, IF(Tracker!F28="offer", 1, 0))))</f>
@@ -6141,11 +6141,11 @@
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85822499999999913</v>
+        <v>0.29392499999999977</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="3"/>
-        <v>0.63572222222222274</v>
+        <v>0.21772222222222259</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -6163,7 +6163,7 @@
       </c>
       <c r="D29">
         <f ca="1">(Tracker!G29+Tracker!H29)/2</f>
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="E29" s="10">
         <f>IF(OR(Tracker!F29="denied",Tracker!F29="on hold",Tracker!F29="No Response",Tracker!F29="pending",Tracker!F53="ghosted"), 0.2, IF(Tracker!F29="interviewing", 0.4, IF(Tracker!F29="rejected", 0.3, IF(Tracker!F29="offer", 1, 0))))</f>
@@ -6186,11 +6186,11 @@
       </c>
       <c r="J29">
         <f t="shared" ca="1" si="2"/>
-        <v>0.96795000000000009</v>
+        <v>-0.19200000000000017</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4340000000000011</v>
+        <v>1.7155555555555555</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -6208,7 +6208,7 @@
       </c>
       <c r="D30">
         <f ca="1">(Tracker!G30+Tracker!H30)/2</f>
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E30" s="10">
         <f>IF(OR(Tracker!F30="denied",Tracker!F30="on hold",Tracker!F30="No Response",Tracker!F30="pending",Tracker!F54="ghosted"), 0.2, IF(Tracker!F30="interviewing", 0.4, IF(Tracker!F30="rejected", 0.3, IF(Tracker!F30="offer", 1, 0))))</f>
@@ -6231,11 +6231,11 @@
       </c>
       <c r="J30">
         <f t="shared" ca="1" si="2"/>
-        <v>0.21554999999999991</v>
+        <v>0.56039999999999957</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15966666666666729</v>
+        <v>0.41511111111111099</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -6253,7 +6253,7 @@
       </c>
       <c r="D31">
         <f ca="1">(Tracker!G31+Tracker!H31)/2</f>
-        <v>77.5</v>
+        <v>106</v>
       </c>
       <c r="E31" s="10">
         <f>IF(OR(Tracker!F31="denied",Tracker!F31="on hold",Tracker!F31="No Response",Tracker!F31="pending",Tracker!F55="ghosted"), 0.2, IF(Tracker!F31="interviewing", 0.4, IF(Tracker!F31="rejected", 0.3, IF(Tracker!F31="offer", 1, 0))))</f>
@@ -6276,11 +6276,11 @@
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.27037500000000003</v>
+        <v>0.6230999999999991</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.20027777777777755</v>
+        <v>0.46155555555555594</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -6298,7 +6298,7 @@
       </c>
       <c r="D32">
         <f ca="1">(Tracker!G32+Tracker!H32)/2</f>
-        <v>99</v>
+        <v>100.5</v>
       </c>
       <c r="E32" s="10">
         <f>IF(OR(Tracker!F32="denied",Tracker!F32="on hold",Tracker!F32="No Response",Tracker!F32="pending",Tracker!F56="ghosted"), 0.2, IF(Tracker!F32="interviewing", 0.4, IF(Tracker!F32="rejected", 0.3, IF(Tracker!F32="offer", 1, 0))))</f>
@@ -6321,11 +6321,11 @@
       </c>
       <c r="J32">
         <f t="shared" ca="1" si="2"/>
-        <v>0.40364999999999984</v>
+        <v>0.45067499999999949</v>
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="3"/>
-        <v>6.9099999999999717E-2</v>
+        <v>0.10044999999999993</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -6343,7 +6343,7 @@
       </c>
       <c r="D33">
         <f ca="1">(Tracker!G33+Tracker!H33)/2</f>
-        <v>104.5</v>
+        <v>115.5</v>
       </c>
       <c r="E33" s="10">
         <f>IF(OR(Tracker!F33="denied",Tracker!F33="on hold",Tracker!F33="No Response",Tracker!F33="pending",Tracker!F57="ghosted"), 0.2, IF(Tracker!F33="interviewing", 0.4, IF(Tracker!F33="rejected", 0.3, IF(Tracker!F33="offer", 1, 0))))</f>
@@ -6366,11 +6366,11 @@
       </c>
       <c r="J33">
         <f t="shared" ca="1" si="2"/>
-        <v>0.57607499999999945</v>
+        <v>0.92092499999999955</v>
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2760749999999996</v>
+        <v>1.6209249999999997</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -6388,7 +6388,7 @@
       </c>
       <c r="D34">
         <f ca="1">(Tracker!G34+Tracker!H34)/2</f>
-        <v>82</v>
+        <v>103.5</v>
       </c>
       <c r="E34" s="10">
         <f>IF(OR(Tracker!F34="denied",Tracker!F34="on hold",Tracker!F34="No Response",Tracker!F34="pending",Tracker!F58="ghosted"), 0.2, IF(Tracker!F34="interviewing", 0.4, IF(Tracker!F34="rejected", 0.3, IF(Tracker!F34="offer", 1, 0))))</f>
@@ -6411,11 +6411,11 @@
       </c>
       <c r="J34">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.12930000000000064</v>
+        <v>0.54472499999999968</v>
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.28619999999999979</v>
+        <v>0.16315000000000079</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -6433,7 +6433,7 @@
       </c>
       <c r="D35">
         <f ca="1">(Tracker!G35+Tracker!H35)/2</f>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E35" s="10">
         <f>IF(OR(Tracker!F35="denied",Tracker!F35="on hold",Tracker!F35="No Response",Tracker!F35="pending",Tracker!F59="ghosted"), 0.2, IF(Tracker!F35="interviewing", 0.4, IF(Tracker!F35="rejected", 0.3, IF(Tracker!F35="offer", 1, 0))))</f>
@@ -6456,11 +6456,11 @@
       </c>
       <c r="J35">
         <f t="shared" ca="1" si="2"/>
-        <v>0.12149999999999972</v>
+        <v>0.15285000000000037</v>
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="3"/>
-        <v>2.4258823529411764</v>
+        <v>2.4750588235294115</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -6478,7 +6478,7 @@
       </c>
       <c r="D36">
         <f ca="1">(Tracker!G36+Tracker!H36)/2</f>
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E36" s="10">
         <f>IF(OR(Tracker!F36="denied",Tracker!F36="on hold",Tracker!F36="No Response",Tracker!F36="pending",Tracker!F60="ghosted"), 0.2, IF(Tracker!F36="interviewing", 0.4, IF(Tracker!F36="rejected", 0.3, IF(Tracker!F36="offer", 1, 0))))</f>
@@ -6501,11 +6501,11 @@
       </c>
       <c r="J36">
         <f t="shared" ca="1" si="2"/>
-        <v>0.84254999999999969</v>
+        <v>0.12149999999999972</v>
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="3"/>
-        <v>0.36169999999999991</v>
+        <v>-0.11900000000000022</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -6523,7 +6523,7 @@
       </c>
       <c r="D37">
         <f ca="1">(Tracker!G37+Tracker!H37)/2</f>
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E37" s="10">
         <f>IF(OR(Tracker!F37="denied",Tracker!F37="on hold",Tracker!F37="No Response",Tracker!F37="pending",Tracker!F61="ghosted"), 0.2, IF(Tracker!F37="interviewing", 0.4, IF(Tracker!F37="rejected", 0.3, IF(Tracker!F37="offer", 1, 0))))</f>
@@ -6546,11 +6546,11 @@
       </c>
       <c r="J37">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68579999999999952</v>
+        <v>0.71714999999999929</v>
       </c>
       <c r="K37">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2572000000000001</v>
+        <v>0.27810000000000024</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="D38">
         <f ca="1">(Tracker!G38+Tracker!H38)/2</f>
-        <v>100.5</v>
+        <v>92</v>
       </c>
       <c r="E38" s="10">
         <f>IF(OR(Tracker!F38="denied",Tracker!F38="on hold",Tracker!F38="No Response",Tracker!F38="pending",Tracker!F62="ghosted"), 0.2, IF(Tracker!F38="interviewing", 0.4, IF(Tracker!F38="rejected", 0.3, IF(Tracker!F38="offer", 1, 0))))</f>
@@ -6591,7 +6591,7 @@
       </c>
       <c r="J38">
         <f t="shared" ca="1" si="2"/>
-        <v>0.45067499999999949</v>
+        <v>0.1841999999999997</v>
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="3"/>
@@ -6613,7 +6613,7 @@
       </c>
       <c r="D39">
         <f ca="1">(Tracker!G39+Tracker!H39)/2</f>
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E39" s="10">
         <f>IF(OR(Tracker!F39="denied",Tracker!F39="on hold",Tracker!F39="No Response",Tracker!F39="pending",Tracker!F63="ghosted"), 0.2, IF(Tracker!F39="interviewing", 0.4, IF(Tracker!F39="rejected", 0.3, IF(Tracker!F39="offer", 1, 0))))</f>
@@ -6636,11 +6636,11 @@
       </c>
       <c r="J39">
         <f t="shared" ca="1" si="2"/>
-        <v>0.37230000000000008</v>
+        <v>-0.22334999999999994</v>
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15600000000000014</v>
+        <v>-0.26199999999999979</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -6658,7 +6658,7 @@
       </c>
       <c r="D40">
         <f ca="1">(Tracker!G40+Tracker!H40)/2</f>
-        <v>94.5</v>
+        <v>99</v>
       </c>
       <c r="E40" s="10">
         <f>IF(OR(Tracker!F40="denied",Tracker!F40="on hold",Tracker!F40="No Response",Tracker!F40="pending",Tracker!F64="ghosted"), 0.2, IF(Tracker!F40="interviewing", 0.4, IF(Tracker!F40="rejected", 0.3, IF(Tracker!F40="offer", 1, 0))))</f>
@@ -6681,11 +6681,11 @@
       </c>
       <c r="J40">
         <f t="shared" ca="1" si="2"/>
-        <v>0.26257499999999956</v>
+        <v>0.40364999999999984</v>
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.4949999999999806E-2</v>
+        <v>6.9099999999999717E-2</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -6703,7 +6703,7 @@
       </c>
       <c r="D41">
         <f ca="1">(Tracker!G41+Tracker!H41)/2</f>
-        <v>95.5</v>
+        <v>100</v>
       </c>
       <c r="E41" s="10">
         <f>IF(OR(Tracker!F41="denied",Tracker!F41="on hold",Tracker!F41="No Response",Tracker!F41="pending",Tracker!F65="ghosted"), 0.2, IF(Tracker!F41="interviewing", 0.4, IF(Tracker!F41="rejected", 0.3, IF(Tracker!F41="offer", 1, 0))))</f>
@@ -6726,11 +6726,11 @@
       </c>
       <c r="J41">
         <f t="shared" ca="1" si="2"/>
-        <v>0.29392499999999977</v>
+        <v>0.43499999999999961</v>
       </c>
       <c r="K41">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.049999999999887E-3</v>
+        <v>8.9999999999999858E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
@@ -6748,7 +6748,7 @@
       </c>
       <c r="D42">
         <f ca="1">(Tracker!G42+Tracker!H42)/2</f>
-        <v>80.5</v>
+        <v>114</v>
       </c>
       <c r="E42" s="10">
         <f>IF(OR(Tracker!F42="denied",Tracker!F42="on hold",Tracker!F42="No Response",Tracker!F42="pending",Tracker!F66="ghosted"), 0.2, IF(Tracker!F42="interviewing", 0.4, IF(Tracker!F42="rejected", 0.3, IF(Tracker!F42="offer", 1, 0))))</f>
@@ -6771,11 +6771,11 @@
       </c>
       <c r="J42">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.17632500000000029</v>
+        <v>0.87389999999999946</v>
       </c>
       <c r="K42">
         <f t="shared" ca="1" si="3"/>
-        <v>0.80408333333333326</v>
+        <v>1.9709999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -6793,7 +6793,7 @@
       </c>
       <c r="D43">
         <f ca="1">(Tracker!G43+Tracker!H43)/2</f>
-        <v>115</v>
+        <v>105.5</v>
       </c>
       <c r="E43" s="10">
         <f>IF(OR(Tracker!F43="denied",Tracker!F43="on hold",Tracker!F43="No Response",Tracker!F43="pending",Tracker!F67="ghosted"), 0.2, IF(Tracker!F43="interviewing", 0.4, IF(Tracker!F43="rejected", 0.3, IF(Tracker!F43="offer", 1, 0))))</f>
@@ -6816,11 +6816,11 @@
       </c>
       <c r="J43">
         <f t="shared" ca="1" si="2"/>
-        <v>0.90525000000000011</v>
+        <v>0.60742499999999966</v>
       </c>
       <c r="K43">
         <f t="shared" ca="1" si="3"/>
-        <v>0.40350000000000019</v>
+        <v>0.20495000000000019</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="D44">
         <f ca="1">(Tracker!G44+Tracker!H44)/2</f>
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E44" s="10">
         <f>IF(OR(Tracker!F44="denied",Tracker!F44="on hold",Tracker!F44="No Response",Tracker!F44="pending",Tracker!F68="ghosted"), 0.2, IF(Tracker!F44="interviewing", 0.4, IF(Tracker!F44="rejected", 0.3, IF(Tracker!F44="offer", 1, 0))))</f>
@@ -6861,11 +6861,11 @@
       </c>
       <c r="J44">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77985000000000015</v>
+        <v>0.68579999999999952</v>
       </c>
       <c r="K44">
         <f t="shared" ca="1" si="3"/>
-        <v>0.31990000000000052</v>
+        <v>0.2572000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
@@ -6883,7 +6883,7 @@
       </c>
       <c r="D45">
         <f ca="1">(Tracker!G45+Tracker!H45)/2</f>
-        <v>110.5</v>
+        <v>111</v>
       </c>
       <c r="E45" s="10">
         <f>IF(OR(Tracker!F45="denied",Tracker!F45="on hold",Tracker!F45="No Response",Tracker!F45="pending",Tracker!F69="ghosted"), 0.2, IF(Tracker!F45="interviewing", 0.4, IF(Tracker!F45="rejected", 0.3, IF(Tracker!F45="offer", 1, 0))))</f>
@@ -6906,11 +6906,11 @@
       </c>
       <c r="J45">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76417499999999983</v>
+        <v>0.77985000000000015</v>
       </c>
       <c r="K45">
         <f t="shared" ca="1" si="3"/>
-        <v>0.30945</v>
+        <v>0.31990000000000052</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
@@ -6928,7 +6928,7 @@
       </c>
       <c r="D46">
         <f ca="1">(Tracker!G46+Tracker!H46)/2</f>
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="E46" s="10">
         <f>IF(OR(Tracker!F46="denied",Tracker!F46="on hold",Tracker!F46="No Response",Tracker!F46="pending",Tracker!F70="ghosted"), 0.2, IF(Tracker!F46="interviewing", 0.4, IF(Tracker!F46="rejected", 0.3, IF(Tracker!F46="offer", 1, 0))))</f>
@@ -6951,11 +6951,11 @@
       </c>
       <c r="J46">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1841999999999997</v>
+        <v>0.5290499999999998</v>
       </c>
       <c r="K46">
         <f t="shared" ca="1" si="3"/>
-        <v>-7.7199999999999491E-2</v>
+        <v>0.15270000000000028</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
@@ -6973,7 +6973,7 @@
       </c>
       <c r="D47">
         <f ca="1">(Tracker!G47+Tracker!H47)/2</f>
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E47" s="10">
         <f>IF(OR(Tracker!F47="denied",Tracker!F47="on hold",Tracker!F47="No Response",Tracker!F47="pending",Tracker!F71="ghosted"), 0.2, IF(Tracker!F47="interviewing", 0.4, IF(Tracker!F47="rejected", 0.3, IF(Tracker!F47="offer", 1, 0))))</f>
@@ -6996,11 +6996,11 @@
       </c>
       <c r="J47">
         <f t="shared" ca="1" si="2"/>
-        <v>0.37230000000000008</v>
+        <v>0.81120000000000081</v>
       </c>
       <c r="K47">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8200000000000465E-2</v>
+        <v>0.34080000000000021</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
@@ -7018,7 +7018,7 @@
       </c>
       <c r="D48">
         <f ca="1">(Tracker!G48+Tracker!H48)/2</f>
-        <v>79.5</v>
+        <v>99</v>
       </c>
       <c r="E48" s="10">
         <f>IF(OR(Tracker!F48="denied",Tracker!F48="on hold",Tracker!F48="No Response",Tracker!F48="pending",Tracker!F72="ghosted"), 0.2, IF(Tracker!F48="interviewing", 0.4, IF(Tracker!F48="rejected", 0.3, IF(Tracker!F48="offer", 1, 0))))</f>
@@ -7041,11 +7041,11 @@
       </c>
       <c r="J48">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.20767500000000005</v>
+        <v>0.40364999999999984</v>
       </c>
       <c r="K48">
         <f t="shared" ca="1" si="3"/>
-        <v>0.49232500000000012</v>
+        <v>1.10365</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
@@ -7063,7 +7063,7 @@
       </c>
       <c r="D49">
         <f ca="1">(Tracker!G49+Tracker!H49)/2</f>
-        <v>113.5</v>
+        <v>86.5</v>
       </c>
       <c r="E49" s="10">
         <f>IF(OR(Tracker!F49="denied",Tracker!F49="on hold",Tracker!F49="No Response",Tracker!F49="pending",Tracker!F73="ghosted"), 0.2, IF(Tracker!F49="interviewing", 0.4, IF(Tracker!F49="rejected", 0.3, IF(Tracker!F49="offer", 1, 0))))</f>
@@ -7086,11 +7086,11 @@
       </c>
       <c r="J49">
         <f t="shared" ca="1" si="2"/>
-        <v>0.85822499999999913</v>
+        <v>1.1775000000000091E-2</v>
       </c>
       <c r="K49">
         <f t="shared" ca="1" si="3"/>
-        <v>0.37215000000000042</v>
+        <v>-0.19214999999999982</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
@@ -7108,7 +7108,7 @@
       </c>
       <c r="D50">
         <f ca="1">(Tracker!G50+Tracker!H50)/2</f>
-        <v>97.5</v>
+        <v>108.5</v>
       </c>
       <c r="E50" s="10">
         <f>IF(OR(Tracker!F50="denied",Tracker!F50="on hold",Tracker!F50="No Response",Tracker!F50="pending",Tracker!F74="ghosted"), 0.2, IF(Tracker!F50="interviewing", 0.4, IF(Tracker!F50="rejected", 0.3, IF(Tracker!F50="offer", 1, 0))))</f>
@@ -7131,11 +7131,11 @@
       </c>
       <c r="J50">
         <f t="shared" ca="1" si="2"/>
-        <v>0.35662500000000019</v>
+        <v>0.70147499999999985</v>
       </c>
       <c r="K50">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0566250000000004</v>
+        <v>1.401475</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
@@ -7153,7 +7153,7 @@
       </c>
       <c r="D51">
         <f ca="1">(Tracker!G51+Tracker!H51)/2</f>
-        <v>84.5</v>
+        <v>104</v>
       </c>
       <c r="E51" s="10">
         <f>IF(OR(Tracker!F51="denied",Tracker!F51="on hold",Tracker!F51="No Response",Tracker!F51="pending",Tracker!F75="ghosted"), 0.2, IF(Tracker!F51="interviewing", 0.4, IF(Tracker!F51="rejected", 0.3, IF(Tracker!F51="offer", 1, 0))))</f>
@@ -7176,11 +7176,11 @@
       </c>
       <c r="J51">
         <f t="shared" ca="1" si="2"/>
-        <v>-5.0924999999999887E-2</v>
+        <v>0.56039999999999957</v>
       </c>
       <c r="K51">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.23394999999999966</v>
+        <v>0.17359999999999998</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
@@ -7198,7 +7198,7 @@
       </c>
       <c r="D52">
         <f ca="1">(Tracker!G52+Tracker!H52)/2</f>
-        <v>110.5</v>
+        <v>94</v>
       </c>
       <c r="E52" s="10">
         <f>IF(OR(Tracker!F52="denied",Tracker!F52="on hold",Tracker!F52="No Response",Tracker!F52="pending",Tracker!F76="ghosted"), 0.2, IF(Tracker!F52="interviewing", 0.4, IF(Tracker!F52="rejected", 0.3, IF(Tracker!F52="offer", 1, 0))))</f>
@@ -7221,11 +7221,11 @@
       </c>
       <c r="J52">
         <f t="shared" ca="1" si="2"/>
-        <v>0.76417499999999983</v>
+        <v>0.24690000000000012</v>
       </c>
       <c r="K52">
         <f t="shared" ca="1" si="3"/>
-        <v>1.464175</v>
+        <v>0.9469000000000003</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
@@ -7243,7 +7243,7 @@
       </c>
       <c r="D53">
         <f ca="1">(Tracker!G53+Tracker!H53)/2</f>
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E53" s="10">
         <f>IF(OR(Tracker!F53="denied",Tracker!F53="on hold",Tracker!F53="No Response",Tracker!F53="pending",Tracker!F77="ghosted"), 0.2, IF(Tracker!F53="interviewing", 0.4, IF(Tracker!F53="rejected", 0.3, IF(Tracker!F53="offer", 1, 0))))</f>
@@ -7266,11 +7266,11 @@
       </c>
       <c r="J53">
         <f t="shared" ca="1" si="2"/>
-        <v>0.37230000000000008</v>
+        <v>0.49770000000000003</v>
       </c>
       <c r="K53">
         <f t="shared" ca="1" si="3"/>
-        <v>2.0964000000000009</v>
+        <v>2.2636000000000012</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="D54">
         <f ca="1">(Tracker!G54+Tracker!H54)/2</f>
-        <v>87.5</v>
+        <v>112.5</v>
       </c>
       <c r="E54" s="10">
         <f>IF(OR(Tracker!F54="denied",Tracker!F54="on hold",Tracker!F54="No Response",Tracker!F54="pending",Tracker!F78="ghosted"), 0.2, IF(Tracker!F54="interviewing", 0.4, IF(Tracker!F54="rejected", 0.3, IF(Tracker!F54="offer", 1, 0))))</f>
@@ -7311,11 +7311,11 @@
       </c>
       <c r="J54">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.20625000000000027</v>
+        <v>0.50624999999999964</v>
       </c>
       <c r="K54">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3250000000000002</v>
+        <v>2.2750000000000004</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
@@ -7333,7 +7333,7 @@
       </c>
       <c r="D55">
         <f ca="1">(Tracker!G55+Tracker!H55)/2</f>
-        <v>94.5</v>
+        <v>115.5</v>
       </c>
       <c r="E55" s="10">
         <f>IF(OR(Tracker!F55="denied",Tracker!F55="on hold",Tracker!F55="No Response",Tracker!F55="pending",Tracker!F79="ghosted"), 0.2, IF(Tracker!F55="interviewing", 0.4, IF(Tracker!F55="rejected", 0.3, IF(Tracker!F55="offer", 1, 0))))</f>
@@ -7356,11 +7356,11 @@
       </c>
       <c r="J55">
         <f t="shared" ca="1" si="2"/>
-        <v>-6.7500000000002558E-3</v>
+        <v>0.59174999999999933</v>
       </c>
       <c r="K55">
         <f t="shared" ca="1" si="3"/>
-        <v>0.69324999999999992</v>
+        <v>1.2917499999999995</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -7378,7 +7378,7 @@
       </c>
       <c r="D56">
         <f ca="1">(Tracker!G56+Tracker!H56)/2</f>
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E56" s="10">
         <f>IF(OR(Tracker!F56="denied",Tracker!F56="on hold",Tracker!F56="No Response",Tracker!F56="pending",Tracker!F80="ghosted"), 0.2, IF(Tracker!F56="interviewing", 0.4, IF(Tracker!F56="rejected", 0.3, IF(Tracker!F56="offer", 1, 0))))</f>
@@ -7401,11 +7401,11 @@
       </c>
       <c r="J56">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.13500000000000023</v>
+        <v>0.2354999999999996</v>
       </c>
       <c r="K56">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.29000000000000026</v>
+        <v>-4.2999999999999927E-2</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
@@ -7423,7 +7423,7 @@
       </c>
       <c r="D57">
         <f ca="1">(Tracker!G57+Tracker!H57)/2</f>
-        <v>92</v>
+        <v>106.5</v>
       </c>
       <c r="E57" s="10">
         <f>IF(OR(Tracker!F57="denied",Tracker!F57="on hold",Tracker!F57="No Response",Tracker!F57="pending",Tracker!F81="ghosted"), 0.2, IF(Tracker!F57="interviewing", 0.4, IF(Tracker!F57="rejected", 0.3, IF(Tracker!F57="offer", 1, 0))))</f>
@@ -7446,11 +7446,11 @@
       </c>
       <c r="J57">
         <f t="shared" ca="1" si="2"/>
-        <v>-7.8000000000000735E-2</v>
+        <v>0.33524999999999983</v>
       </c>
       <c r="K57">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.252</v>
+        <v>2.3499999999999854E-2</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
@@ -7468,7 +7468,7 @@
       </c>
       <c r="D58">
         <f ca="1">(Tracker!G58+Tracker!H58)/2</f>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E58" s="10">
         <f>IF(OR(Tracker!F58="denied",Tracker!F58="on hold",Tracker!F58="No Response",Tracker!F58="pending",Tracker!F82="ghosted"), 0.2, IF(Tracker!F58="interviewing", 0.4, IF(Tracker!F58="rejected", 0.3, IF(Tracker!F58="offer", 1, 0))))</f>
@@ -7491,11 +7491,11 @@
       </c>
       <c r="J58">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.24900000000000055</v>
+        <v>-0.16350000000000042</v>
       </c>
       <c r="K58">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.3660000000000001</v>
+        <v>-0.30899999999999994</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="D59">
         <f ca="1">(Tracker!G59+Tracker!H59)/2</f>
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E59" s="10">
         <f>IF(OR(Tracker!F59="denied",Tracker!F59="on hold",Tracker!F59="No Response",Tracker!F59="pending",Tracker!F83="ghosted"), 0.2, IF(Tracker!F59="interviewing", 0.4, IF(Tracker!F59="rejected", 0.3, IF(Tracker!F59="offer", 1, 0))))</f>
@@ -7536,11 +7536,11 @@
       </c>
       <c r="J59">
         <f t="shared" ca="1" si="2"/>
-        <v>0.43499999999999961</v>
+        <v>0.29249999999999954</v>
       </c>
       <c r="K59">
         <f t="shared" ca="1" si="3"/>
-        <v>8.9999999999999858E-2</v>
+        <v>-5.0000000000001155E-3</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
@@ -7558,7 +7558,7 @@
       </c>
       <c r="D60">
         <f ca="1">(Tracker!G60+Tracker!H60)/2</f>
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="E60" s="10">
         <f>IF(OR(Tracker!F60="denied",Tracker!F60="on hold",Tracker!F60="No Response",Tracker!F60="pending",Tracker!F84="ghosted"), 0.2, IF(Tracker!F60="interviewing", 0.4, IF(Tracker!F60="rejected", 0.3, IF(Tracker!F60="offer", 1, 0))))</f>
@@ -7581,11 +7581,11 @@
       </c>
       <c r="J60">
         <f t="shared" ca="1" si="2"/>
-        <v>0.37799999999999967</v>
+        <v>0.71999999999999931</v>
       </c>
       <c r="K60">
         <f t="shared" ca="1" si="3"/>
-        <v>5.2000000000000046E-2</v>
+        <v>0.2799999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
@@ -7603,7 +7603,7 @@
       </c>
       <c r="D61">
         <f ca="1">(Tracker!G61+Tracker!H61)/2</f>
-        <v>96.5</v>
+        <v>106</v>
       </c>
       <c r="E61" s="10">
         <f>IF(OR(Tracker!F61="denied",Tracker!F61="on hold",Tracker!F61="No Response",Tracker!F61="pending",Tracker!F85="ghosted"), 0.2, IF(Tracker!F61="interviewing", 0.4, IF(Tracker!F61="rejected", 0.3, IF(Tracker!F61="offer", 1, 0))))</f>
@@ -7626,11 +7626,11 @@
       </c>
       <c r="J61">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0249999999999684E-2</v>
+        <v>0.32099999999999973</v>
       </c>
       <c r="K61">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.16649999999999987</v>
+        <v>1.4000000000000234E-2</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
@@ -7648,7 +7648,7 @@
       </c>
       <c r="D62">
         <f ca="1">(Tracker!G62+Tracker!H62)/2</f>
-        <v>85.5</v>
+        <v>101</v>
       </c>
       <c r="E62" s="10">
         <f>IF(OR(Tracker!F62="denied",Tracker!F62="on hold",Tracker!F62="No Response",Tracker!F62="pending",Tracker!F86="ghosted"), 0.2, IF(Tracker!F62="interviewing", 0.4, IF(Tracker!F62="rejected", 0.3, IF(Tracker!F62="offer", 1, 0))))</f>
@@ -7671,11 +7671,11 @@
       </c>
       <c r="J62">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.26325000000000065</v>
+        <v>0.17849999999999966</v>
       </c>
       <c r="K62">
         <f t="shared" ca="1" si="3"/>
-        <v>0.43674999999999953</v>
+        <v>0.87849999999999984</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
@@ -7693,7 +7693,7 @@
       </c>
       <c r="D63">
         <f ca="1">(Tracker!G63+Tracker!H63)/2</f>
-        <v>119</v>
+        <v>87.5</v>
       </c>
       <c r="E63" s="10">
         <f>IF(OR(Tracker!F63="denied",Tracker!F63="on hold",Tracker!F63="No Response",Tracker!F63="pending",Tracker!F87="ghosted"), 0.2, IF(Tracker!F63="interviewing", 0.4, IF(Tracker!F63="rejected", 0.3, IF(Tracker!F63="offer", 1, 0))))</f>
@@ -7716,11 +7716,11 @@
       </c>
       <c r="J63">
         <f t="shared" ca="1" si="2"/>
-        <v>0.69149999999999912</v>
+        <v>-0.20625000000000027</v>
       </c>
       <c r="K63">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26100000000000012</v>
+        <v>-0.33749999999999991</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="D64">
         <f ca="1">(Tracker!G64+Tracker!H64)/2</f>
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="E64" s="10">
         <f>IF(OR(Tracker!F64="denied",Tracker!F64="on hold",Tracker!F64="No Response",Tracker!F64="pending",Tracker!F88="ghosted"), 0.2, IF(Tracker!F64="interviewing", 0.4, IF(Tracker!F64="rejected", 0.3, IF(Tracker!F64="offer", 1, 0))))</f>
@@ -7761,11 +7761,11 @@
       </c>
       <c r="J64">
         <f t="shared" ca="1" si="2"/>
-        <v>-7.8000000000000735E-2</v>
+        <v>0.37799999999999967</v>
       </c>
       <c r="K64">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.252</v>
+        <v>5.2000000000000046E-2</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
@@ -7783,7 +7783,7 @@
       </c>
       <c r="D65">
         <f ca="1">(Tracker!G65+Tracker!H65)/2</f>
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E65" s="10">
         <f>IF(OR(Tracker!F65="denied",Tracker!F65="on hold",Tracker!F65="No Response",Tracker!F65="pending",Tracker!F89="ghosted"), 0.2, IF(Tracker!F65="interviewing", 0.4, IF(Tracker!F65="rejected", 0.3, IF(Tracker!F65="offer", 1, 0))))</f>
@@ -7806,11 +7806,11 @@
       </c>
       <c r="J65">
         <f t="shared" ca="1" si="2"/>
-        <v>0.3523499999999995</v>
+        <v>4.4549999999999645E-2</v>
       </c>
       <c r="K65">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4899999999999931E-2</v>
+        <v>-0.1702999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
@@ -7828,7 +7828,7 @@
       </c>
       <c r="D66">
         <f ca="1">(Tracker!G66+Tracker!H66)/2</f>
-        <v>113</v>
+        <v>103.5</v>
       </c>
       <c r="E66" s="10">
         <f>IF(OR(Tracker!F66="denied",Tracker!F66="on hold",Tracker!F66="No Response",Tracker!F66="pending",Tracker!F90="ghosted"), 0.2, IF(Tracker!F66="interviewing", 0.4, IF(Tracker!F66="rejected", 0.3, IF(Tracker!F66="offer", 1, 0))))</f>
@@ -7851,11 +7851,11 @@
       </c>
       <c r="J66">
         <f t="shared" ca="1" si="2"/>
-        <v>0.19844999999999935</v>
+        <v>-4.5225000000000293E-2</v>
       </c>
       <c r="K66">
         <f t="shared" ca="1" si="3"/>
-        <v>1.0671428571428581</v>
+        <v>0.80928571428571461</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
@@ -7873,7 +7873,7 @@
       </c>
       <c r="D67">
         <f ca="1">(Tracker!G67+Tracker!H67)/2</f>
-        <v>88</v>
+        <v>111.5</v>
       </c>
       <c r="E67" s="10">
         <f>IF(OR(Tracker!F67="denied",Tracker!F67="on hold",Tracker!F67="No Response",Tracker!F67="pending",Tracker!F91="ghosted"), 0.2, IF(Tracker!F67="interviewing", 0.4, IF(Tracker!F67="rejected", 0.3, IF(Tracker!F67="offer", 1, 0))))</f>
@@ -7896,11 +7896,11 @@
       </c>
       <c r="J67">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.44280000000000053</v>
+        <v>0.15997499999999931</v>
       </c>
       <c r="K67">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.32800000000000007</v>
+        <v>0.11849999999999961</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
@@ -7918,7 +7918,7 @@
       </c>
       <c r="D68">
         <f ca="1">(Tracker!G68+Tracker!H68)/2</f>
-        <v>89</v>
+        <v>94.5</v>
       </c>
       <c r="E68" s="10">
         <f>IF(OR(Tracker!F68="denied",Tracker!F68="on hold",Tracker!F68="No Response",Tracker!F68="pending",Tracker!F92="ghosted"), 0.2, IF(Tracker!F68="interviewing", 0.4, IF(Tracker!F68="rejected", 0.3, IF(Tracker!F68="offer", 1, 0))))</f>
@@ -7941,11 +7941,11 @@
       </c>
       <c r="J68">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.41715000000000035</v>
+        <v>-0.27607500000000051</v>
       </c>
       <c r="K68">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.30900000000000016</v>
+        <v>-0.2044999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
@@ -7963,7 +7963,7 @@
       </c>
       <c r="D69">
         <f ca="1">(Tracker!G69+Tracker!H69)/2</f>
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="E69" s="10">
         <f>IF(OR(Tracker!F69="denied",Tracker!F69="on hold",Tracker!F69="No Response",Tracker!F69="pending",Tracker!F93="ghosted"), 0.2, IF(Tracker!F69="interviewing", 0.4, IF(Tracker!F69="rejected", 0.3, IF(Tracker!F69="offer", 1, 0))))</f>
@@ -7986,11 +7986,11 @@
       </c>
       <c r="J69">
         <f t="shared" ca="1" si="2"/>
-        <v>0.27539999999999942</v>
+        <v>-0.49409999999999998</v>
       </c>
       <c r="K69">
         <f t="shared" ca="1" si="3"/>
-        <v>0.20400000000000018</v>
+        <v>-0.3660000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
@@ -8008,7 +8008,7 @@
       </c>
       <c r="D70">
         <f ca="1">(Tracker!G70+Tracker!H70)/2</f>
-        <v>92</v>
+        <v>79.5</v>
       </c>
       <c r="E70" s="10">
         <f>IF(OR(Tracker!F70="denied",Tracker!F70="on hold",Tracker!F70="No Response",Tracker!F70="pending",Tracker!F94="ghosted"), 0.2, IF(Tracker!F70="interviewing", 0.4, IF(Tracker!F70="rejected", 0.3, IF(Tracker!F70="offer", 1, 0))))</f>
@@ -8031,11 +8031,11 @@
       </c>
       <c r="J70">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.34020000000000028</v>
+        <v>-0.66082500000000044</v>
       </c>
       <c r="K70">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.25199999999999978</v>
+        <v>-0.48950000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>